<commit_message>
Data Update for 13-04-2020
</commit_message>
<xml_diff>
--- a/source-xlsx/13-04-2020.xlsx
+++ b/source-xlsx/13-04-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\covid19\source-xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C66AE7-667F-4EDD-84B0-F35927B63B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68682C1F-3DB9-4894-8C9E-04266A90A189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="132">
   <si>
     <t>division</t>
   </si>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124:XFD167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -829,7 +829,9 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
@@ -839,7 +841,9 @@
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -849,7 +853,9 @@
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -859,7 +865,9 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="5"/>
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -869,7 +877,9 @@
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="5"/>
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
@@ -879,7 +889,9 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
@@ -889,7 +901,9 @@
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="5"/>
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
@@ -899,7 +913,9 @@
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="5"/>
+      <c r="A10" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -909,7 +925,9 @@
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
@@ -919,7 +937,9 @@
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
@@ -929,7 +949,9 @@
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
@@ -951,7 +973,9 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
@@ -961,7 +985,9 @@
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
@@ -971,7 +997,9 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
@@ -981,7 +1009,9 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>22</v>
       </c>
@@ -991,7 +1021,9 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1013,7 +1045,9 @@
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
@@ -1023,7 +1057,9 @@
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
@@ -1033,7 +1069,9 @@
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="B23" s="3" t="s">
         <v>28</v>
       </c>
@@ -1055,7 +1093,9 @@
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B25" s="3" t="s">
         <v>31</v>
       </c>
@@ -1065,7 +1105,9 @@
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
@@ -1075,7 +1117,9 @@
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
@@ -1085,7 +1129,9 @@
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="7"/>
+      <c r="A28" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B28" s="3" t="s">
         <v>34</v>
       </c>
@@ -1119,7 +1165,9 @@
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="7"/>
+      <c r="A31" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="B31" s="3" t="s">
         <v>38</v>
       </c>
@@ -1129,7 +1177,9 @@
       <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="7"/>
+      <c r="A32" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="B32" s="3" t="s">
         <v>39</v>
       </c>
@@ -1139,7 +1189,9 @@
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="7"/>
+      <c r="A33" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1161,7 +1213,9 @@
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="7"/>
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="B35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1171,7 +1225,9 @@
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="7"/>
+      <c r="A36" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="B36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1181,7 +1237,9 @@
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="7"/>
+      <c r="A37" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="B37" s="3" t="s">
         <v>44</v>
       </c>

</xml_diff>